<commit_message>
[CONC] Work review fine points
</commit_message>
<xml_diff>
--- a/resources/Imagens_Diagramas_Tabelas_1.2.0.xlsx
+++ b/resources/Imagens_Diagramas_Tabelas_1.2.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="19155" windowHeight="8505" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19155" windowHeight="8505" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="Plan4" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
     <sheet name="Plan5" sheetId="7" r:id="rId7"/>
+    <sheet name="Plan6" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -3970,6 +3971,1177 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>136072</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>190343</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>544287</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="75" name="Grupo 74"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="748393" y="761843"/>
+          <a:ext cx="8368394" cy="6014514"/>
+          <a:chOff x="748393" y="761843"/>
+          <a:chExt cx="8368394" cy="6014514"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="2" name="Retângulo 1"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2256346" y="761843"/>
+            <a:ext cx="2036989" cy="600075"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1600" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>1. Disponibilizar</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1600" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t> treinamento</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1600" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="Retângulo 2"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5510861" y="1499347"/>
+            <a:ext cx="2036989" cy="600075"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1600" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>2. Plano de Qualidade</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="Retângulo 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2694196" y="2543174"/>
+            <a:ext cx="2039711" cy="600075"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1600" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>3. Avaliação do Produto</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Retângulo 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5508154" y="2552699"/>
+            <a:ext cx="2036989" cy="600075"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1600" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>4. Avaliação do Processo</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="11" name="Conector angulado 10"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="3" idx="2"/>
+            <a:endCxn id="8" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000">
+            <a:off x="4899828" y="913646"/>
+            <a:ext cx="443752" cy="2815304"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 50000"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln w="31750" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:tailEnd type="none"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="12" name="Conector angulado 11"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="3" idx="2"/>
+            <a:endCxn id="9" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000">
+            <a:off x="6301365" y="2324707"/>
+            <a:ext cx="453277" cy="2707"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 50000"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln w="31750" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:tailEnd type="none"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="15" name="Retângulo 14"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4159686" y="3562349"/>
+            <a:ext cx="2036989" cy="600075"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1600" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>5. Relatório de não conformidades</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="16" name="Conector angulado 15"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="8" idx="2"/>
+            <a:endCxn id="15" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="4235885" y="2621415"/>
+            <a:ext cx="419100" cy="1462768"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 50000"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln w="31750" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:tailEnd type="none"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="19" name="Conector angulado 18"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="9" idx="2"/>
+            <a:endCxn id="15" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000">
+            <a:off x="5647628" y="2681967"/>
+            <a:ext cx="409575" cy="1351189"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 50000"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln w="31750" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:tailEnd type="none"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="26" name="Retângulo 25"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4155203" y="4425204"/>
+            <a:ext cx="2036989" cy="600075"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1600" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>7. Aprovar produto final</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="27" name="Conector reto 26"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="15" idx="2"/>
+            <a:endCxn id="26" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="5170096" y="4162424"/>
+            <a:ext cx="4483" cy="262780"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:tailEnd type="none"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="30" name="Retângulo 29"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7857005" y="2552699"/>
+            <a:ext cx="1259782" cy="2808515"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1600" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>6. Relatório periódico</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="32" name="Conector angulado 31"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="3" idx="2"/>
+            <a:endCxn id="30" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="7281488" y="1347290"/>
+            <a:ext cx="453277" cy="1957540"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 50000"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln w="31750" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:tailEnd type="none"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="35" name="Retângulo 34"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4150719" y="5294788"/>
+            <a:ext cx="2036989" cy="600075"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1600" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>8. Relatório de lições aprendidas</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="36" name="Conector reto 35"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="26" idx="2"/>
+            <a:endCxn id="35" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="5165612" y="5025279"/>
+            <a:ext cx="4484" cy="269509"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:tailEnd type="none"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="43" name="Forma 42"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="2" idx="3"/>
+            <a:endCxn id="3" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4293335" y="1061881"/>
+            <a:ext cx="1217526" cy="737504"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 50000"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln w="31750" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:tailEnd type="none"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="44" name="Retângulo 43"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="748393" y="2530921"/>
+            <a:ext cx="1483178" cy="2830285"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1600" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>9. Suporte aos envolvidos no Projeto</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="45" name="Forma 44"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="2" idx="1"/>
+            <a:endCxn id="44" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="10800000" flipV="1">
+            <a:off x="1489982" y="1061881"/>
+            <a:ext cx="766364" cy="1469040"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector2">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:tailEnd type="none"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="48" name="Forma 47"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="44" idx="2"/>
+            <a:endCxn id="51" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="2632977" y="4218211"/>
+            <a:ext cx="1217848" cy="3503838"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector2">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:tailEnd type="none"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="51" name="Fluxograma: Conector 50"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4993820" y="6381750"/>
+            <a:ext cx="353786" cy="394607"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:tailEnd type="none"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:endParaRPr lang="pt-BR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="53" name="Forma 52"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="30" idx="2"/>
+            <a:endCxn id="51" idx="6"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000">
+            <a:off x="6308331" y="4400489"/>
+            <a:ext cx="1217840" cy="3139290"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector2">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:tailEnd type="none"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="56" name="Forma 55"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="35" idx="2"/>
+            <a:endCxn id="51" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="4926520" y="6137556"/>
+            <a:ext cx="486887" cy="1499"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 50000"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln w="31750" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:tailEnd type="none"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -4776,8 +5948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" activeCellId="1" sqref="D7 F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4895,4 +6067,19 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>